<commit_message>
Atualização gráficos e arquivos
</commit_message>
<xml_diff>
--- a/ExecucoesGerais/novo__AGEO2_vs_AGEOsvar5.xlsx
+++ b/ExecucoesGerais/novo__AGEO2_vs_AGEOsvar5.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19485" windowHeight="7905" activeTab="4"/>
+    <workbookView windowWidth="14460" windowHeight="7905" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="GRI" sheetId="1" r:id="rId1"/>
@@ -79,8 +79,8 @@
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -88,29 +88,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -122,39 +99,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -169,6 +131,28 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -176,14 +160,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -198,6 +182,37 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -206,15 +221,7 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -222,14 +229,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -241,36 +241,6 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -286,7 +256,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -298,7 +292,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -310,7 +340,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -322,109 +424,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -447,6 +447,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -463,31 +487,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -513,25 +522,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -540,152 +540,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -693,6 +693,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -9849,9 +9852,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
+      <xdr:colOff>146685</xdr:colOff>
       <xdr:row>56</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -9860,7 +9863,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="685800" y="7423150"/>
-        <a:ext cx="4114800" cy="2743200"/>
+        <a:ext cx="4128135" cy="2806700"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -14077,7 +14080,7 @@
   <sheetPr/>
   <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="A58" sqref="A58:H66"/>
     </sheetView>
   </sheetViews>
@@ -14668,15 +14671,16 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I68"/>
+  <dimension ref="A1:K68"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C40" sqref="A1:C40"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="3" width="12.625"/>
+    <col min="8" max="11" width="12.625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -14701,7 +14705,7 @@
         <v>532.219616022656</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:11">
       <c r="A3" s="1">
         <v>50</v>
       </c>
@@ -14711,8 +14715,11 @@
       <c r="C3" s="1">
         <v>5.68517205506138</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="1">
         <v>100</v>
       </c>
@@ -14722,8 +14729,11 @@
       <c r="C4" s="1">
         <v>1.92498087391738</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="1">
         <v>500</v>
       </c>
@@ -14733,8 +14743,12 @@
       <c r="C5" s="1">
         <v>0.913692728642571</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="1">
         <v>1000</v>
       </c>
@@ -14744,6 +14758,8 @@
       <c r="C6" s="1">
         <v>0.569016046850113</v>
       </c>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1">
@@ -14965,7 +14981,7 @@
         <v>0.00310540050405335</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:11">
       <c r="A27" s="1">
         <v>35000</v>
       </c>
@@ -14975,8 +14991,9 @@
       <c r="C27" s="1">
         <v>0.00208124786280879</v>
       </c>
-    </row>
-    <row r="28" spans="1:3">
+      <c r="K27" s="3"/>
+    </row>
+    <row r="28" spans="1:11">
       <c r="A28" s="1">
         <v>40000</v>
       </c>
@@ -14986,8 +15003,9 @@
       <c r="C28" s="1">
         <v>0.00200036539377556</v>
       </c>
-    </row>
-    <row r="29" spans="1:3">
+      <c r="K28" s="3"/>
+    </row>
+    <row r="29" spans="1:11">
       <c r="A29" s="1">
         <v>45000</v>
       </c>
@@ -14997,8 +15015,9 @@
       <c r="C29" s="1">
         <v>0.00100927905315727</v>
       </c>
-    </row>
-    <row r="30" spans="1:3">
+      <c r="K29" s="3"/>
+    </row>
+    <row r="30" spans="1:11">
       <c r="A30" s="1">
         <v>50000</v>
       </c>
@@ -15008,8 +15027,9 @@
       <c r="C30" s="1">
         <v>0.000985142821608248</v>
       </c>
-    </row>
-    <row r="31" spans="1:3">
+      <c r="K30" s="3"/>
+    </row>
+    <row r="31" spans="1:11">
       <c r="A31" s="1">
         <v>55000</v>
       </c>
@@ -15019,8 +15039,9 @@
       <c r="C31" s="1">
         <v>0.00080860127135773</v>
       </c>
-    </row>
-    <row r="32" spans="1:3">
+      <c r="K31" s="3"/>
+    </row>
+    <row r="32" spans="1:11">
       <c r="A32" s="1">
         <v>60000</v>
       </c>
@@ -15030,8 +15051,10 @@
       <c r="C32" s="1">
         <v>0.000585890539301531</v>
       </c>
-    </row>
-    <row r="33" spans="1:3">
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+    </row>
+    <row r="33" spans="1:11">
       <c r="A33" s="1">
         <v>65000</v>
       </c>
@@ -15041,8 +15064,10 @@
       <c r="C33" s="1">
         <v>0.000494042431269608</v>
       </c>
-    </row>
-    <row r="34" spans="1:3">
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+    </row>
+    <row r="34" spans="1:11">
       <c r="A34" s="1">
         <v>70000</v>
       </c>
@@ -15052,8 +15077,10 @@
       <c r="C34" s="1">
         <v>0.000480809039745232</v>
       </c>
-    </row>
-    <row r="35" spans="1:3">
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+    </row>
+    <row r="35" spans="1:11">
       <c r="A35" s="1">
         <v>75000</v>
       </c>
@@ -15063,8 +15090,10 @@
       <c r="C35" s="1">
         <v>0.00044873289657446</v>
       </c>
-    </row>
-    <row r="36" spans="1:3">
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+    </row>
+    <row r="36" spans="1:11">
       <c r="A36" s="1">
         <v>80000</v>
       </c>
@@ -15074,8 +15103,10 @@
       <c r="C36" s="1">
         <v>0.000400772394705883</v>
       </c>
-    </row>
-    <row r="37" spans="1:3">
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+    </row>
+    <row r="37" spans="1:11">
       <c r="A37" s="1">
         <v>85000</v>
       </c>
@@ -15085,8 +15116,10 @@
       <c r="C37" s="1">
         <v>0.000400772394705883</v>
       </c>
-    </row>
-    <row r="38" spans="1:3">
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+    </row>
+    <row r="38" spans="1:11">
       <c r="A38" s="1">
         <v>90000</v>
       </c>
@@ -15096,8 +15129,10 @@
       <c r="C38" s="1">
         <v>0.000389836563451008</v>
       </c>
-    </row>
-    <row r="39" spans="1:3">
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+    </row>
+    <row r="39" spans="1:11">
       <c r="A39" s="1">
         <v>95000</v>
       </c>
@@ -15107,8 +15142,10 @@
       <c r="C39" s="1">
         <v>0.000383723668423885</v>
       </c>
-    </row>
-    <row r="40" spans="1:3">
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+    </row>
+    <row r="40" spans="1:11">
       <c r="A40" s="1">
         <v>100000</v>
       </c>
@@ -15118,6 +15155,9 @@
       <c r="C40" s="1">
         <v>0.000117880494477845</v>
       </c>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
     </row>
     <row r="58" spans="1:9">
       <c r="A58" s="1" t="s">

</xml_diff>